<commit_message>
Added to SQL Translations spreadsheet. Made major progress on Live Plot vi.
</commit_message>
<xml_diff>
--- a/Database2.0/SQL Column Translations.xlsx
+++ b/Database2.0/SQL Column Translations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="14310"/>
+    <workbookView xWindow="-13845" yWindow="1800" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dust_event" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>File Location</t>
   </si>
@@ -66,13 +66,16 @@
   </si>
   <si>
     <t>Highest-Lowest dust event quality</t>
+  </si>
+  <si>
+    <t>&lt;- Andrew's Code should never run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,18 +104,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -191,6 +202,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -225,6 +237,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,14 +413,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -415,31 +428,31 @@
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -453,7 +466,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -467,7 +480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-2</v>
       </c>
@@ -481,7 +494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-3</v>
       </c>
@@ -495,7 +508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-4</v>
       </c>
@@ -509,7 +522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-5</v>
       </c>
@@ -533,46 +546,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -585,8 +599,11 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -599,8 +616,9 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-2</v>
       </c>
@@ -614,7 +632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-3</v>
       </c>
@@ -628,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-4</v>
       </c>
@@ -642,7 +660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-5</v>
       </c>
@@ -657,9 +675,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Much improved small acc compatibility.
</commit_message>
<xml_diff>
--- a/Database2.0/SQL Column Translations.xlsx
+++ b/Database2.0/SQL Column Translations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-13845" yWindow="1800" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="-13845" yWindow="1800" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="dust_event" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>File Location</t>
   </si>
@@ -69,13 +69,16 @@
   </si>
   <si>
     <t>&lt;- Andrew's Code should never run</t>
+  </si>
+  <si>
+    <t>IDL Batch Processor failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,7 +205,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,7 +239,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,14 +414,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -428,7 +429,7 @@
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -438,7 +439,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -452,7 +453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>0</v>
       </c>
@@ -466,7 +467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -480,7 +481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>-2</v>
       </c>
@@ -494,7 +495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>-3</v>
       </c>
@@ -508,7 +509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>-4</v>
       </c>
@@ -522,7 +523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>-5</v>
       </c>
@@ -533,7 +534,7 @@
         <v>-5</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -546,14 +547,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -562,7 +563,7 @@
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -572,7 +573,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -586,7 +587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>0</v>
       </c>
@@ -603,7 +604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -618,7 +619,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>-2</v>
       </c>
@@ -632,7 +633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>-3</v>
       </c>
@@ -646,7 +647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>-4</v>
       </c>
@@ -660,7 +661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>-5</v>
       </c>

</xml_diff>

<commit_message>
Finalized modifications to batch processing.
</commit_message>
<xml_diff>
--- a/Database2.0/SQL Column Translations.xlsx
+++ b/Database2.0/SQL Column Translations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-13845" yWindow="1800" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="-13845" yWindow="1800" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dust_event" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>File Location</t>
   </si>
@@ -23,21 +23,6 @@
     <t>Storage</t>
   </si>
   <si>
-    <t>Local Cache</t>
-  </si>
-  <si>
-    <t>Retry Labview Files</t>
-  </si>
-  <si>
-    <t>Labview Files</t>
-  </si>
-  <si>
-    <t>Writing from Queue</t>
-  </si>
-  <si>
-    <t>IDL Processing</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -72,13 +57,16 @@
   </si>
   <si>
     <t>IDL Batch Processor failed</t>
+  </si>
+  <si>
+    <t>Processing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +193,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -239,6 +228,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -414,14 +404,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -429,17 +419,17 @@
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -447,94 +437,70 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-1</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>-2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>-2</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>-3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>-3</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>-4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>-4</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>-5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>-5</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -547,14 +513,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -563,17 +529,17 @@
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -581,98 +547,74 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-1</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>-2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>-2</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>-3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>-3</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>-4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>-4</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>-5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>-5</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>